<commit_message>
Commit 047 -> Añadido documentación y enlace a este repositorio.
</commit_message>
<xml_diff>
--- a/Documentación/ResumenEntregaTrabajoTSI.xlsx
+++ b/Documentación/ResumenEntregaTrabajoTSI.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Dropbox\UPO\3-ano\1-Cuatrimestre\Tecnologías de Sistemas de Información\Trabajo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Dropbox\UPO\3-ano\1-Cuatrimestre\Tecnologías de Sistemas de Información\Trabajo\Empresa-gestora-de-espacios-teatrales-Odoo-11\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83F3E12-9754-4EAA-A91A-B1B8D9D8EABA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE0402C4-23A0-4F47-ACD1-714594AC00BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PLANTILLA ENTREGA" sheetId="1" r:id="rId1"/>
@@ -549,7 +549,7 @@
   <dimension ref="B3:O32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D23" sqref="D23:L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1327,6 +1327,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>